<commit_message>
actualización de la programación de cron para ejecutar cada 30 minutos y actualización de archivos de entrada y salida
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -1,40 +1,54 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://corpsmu-my.sharepoint.com/personal/dcea_smu_cl/Documents/Automatizacion_SAC/GitHub Respository/zclient-banking-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_AD4D2F04E46CFB4ACB3E207DB5D5F69A693EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27124917-9F3D-42F2-B68D-8EBE77B5D863}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_AD4D2F04E46CFB4ACB3E207DB5D5F69A693EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9250B86-1C05-460B-AFC4-DB05328CF8A8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>mail</t>
   </si>
+  <si>
+    <t>contacto.diego.c@gmail.com</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -345,17 +359,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>